<commit_message>
update db y score
</commit_message>
<xml_diff>
--- a/Score.xlsx
+++ b/Score.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\credistar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Score!$B$1:$D$117</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="144">
   <si>
     <t>Menor de 30</t>
   </si>
@@ -370,12 +376,99 @@
   </si>
   <si>
     <t>Puntos de corte</t>
+  </si>
+  <si>
+    <t>socres</t>
+  </si>
+  <si>
+    <t>entidad_id</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>regla_edad</t>
+  </si>
+  <si>
+    <t>REGLA</t>
+  </si>
+  <si>
+    <t>TIPO DE REGLA</t>
+  </si>
+  <si>
+    <t>VALIDACION</t>
+  </si>
+  <si>
+    <t>PUNTAJE</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>DEPENDIENTES</t>
+  </si>
+  <si>
+    <t>TRABAJO</t>
+  </si>
+  <si>
+    <t>CREDITO</t>
+  </si>
+  <si>
+    <t>OTRO</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>BUENO</t>
+  </si>
+  <si>
+    <t>CIA</t>
+  </si>
+  <si>
+    <t>DIUNSA</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>IDENTIDAD</t>
+  </si>
+  <si>
+    <t>ARMANDO</t>
+  </si>
+  <si>
+    <t>DEPENDIENTE</t>
+  </si>
+  <si>
+    <t>&gt;20</t>
+  </si>
+  <si>
+    <t>&gt;25</t>
+  </si>
+  <si>
+    <t>EXCELENTE</t>
+  </si>
+  <si>
+    <t>TOTAL SCORE</t>
+  </si>
+  <si>
+    <t>fecah</t>
+  </si>
+  <si>
+    <t>;l';;;;;;;;;;;;;;;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +545,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -471,6 +564,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -479,6 +579,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -804,19 +912,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -833,7 +941,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -848,7 +956,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -863,7 +971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,7 +980,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -881,7 +989,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -890,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -899,7 +1007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -908,7 +1016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -917,7 +1025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -926,7 +1034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -935,7 +1043,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
@@ -946,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -957,7 +1065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -966,7 +1074,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -975,7 +1083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -984,7 +1092,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -993,7 +1101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1004,7 +1112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
@@ -1036,8 +1144,14 @@
       <c r="D21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="H21" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1047,8 +1161,11 @@
       <c r="D22" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="J22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1056,8 +1173,14 @@
       <c r="D23" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="J23" t="s">
+        <v>118</v>
+      </c>
+      <c r="K23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
@@ -1068,7 +1191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -1077,7 +1200,7 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1088,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1104,7 +1227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1126,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1148,7 +1271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1162,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1173,7 +1296,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1184,7 +1307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1195,7 +1318,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1217,7 +1340,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>37</v>
       </c>
@@ -1228,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +1373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>40</v>
       </c>
@@ -1261,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>41</v>
       </c>
@@ -1272,7 +1395,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>42</v>
       </c>
@@ -1283,7 +1406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1297,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
         <v>43</v>
       </c>
@@ -1308,7 +1431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>45</v>
       </c>
@@ -1330,7 +1453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>46</v>
       </c>
@@ -1341,7 +1464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>47</v>
       </c>
@@ -1350,7 +1473,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>48</v>
       </c>
@@ -1359,7 +1482,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="2:4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>49</v>
       </c>
@@ -1370,7 +1493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="2:4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>50</v>
       </c>
@@ -1381,7 +1504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="2:4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>51</v>
       </c>
@@ -1390,7 +1513,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="2:4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>52</v>
       </c>
@@ -1399,7 +1522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
         <v>53</v>
       </c>
@@ -1410,7 +1533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="2:4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>54</v>
       </c>
@@ -1421,7 +1544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="2:4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>55</v>
       </c>
@@ -1432,7 +1555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>56</v>
       </c>
@@ -1441,7 +1564,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="2:4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>57</v>
       </c>
@@ -1452,7 +1575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="2:4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>58</v>
       </c>
@@ -1463,7 +1586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="2:4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>59</v>
       </c>
@@ -1472,7 +1595,7 @@
       </c>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="2:4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>60</v>
       </c>
@@ -1481,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>61</v>
       </c>
@@ -1490,7 +1613,7 @@
       </c>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>62</v>
       </c>
@@ -1501,7 +1624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>63</v>
       </c>
@@ -1510,7 +1633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>64</v>
       </c>
@@ -1521,7 +1644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>31</v>
       </c>
@@ -1532,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>65</v>
       </c>
@@ -1541,7 +1664,7 @@
       </c>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>66</v>
       </c>
@@ -1552,7 +1675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>67</v>
       </c>
@@ -1563,7 +1686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>68</v>
       </c>
@@ -1574,7 +1697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>6</v>
       </c>
@@ -1588,7 +1711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>69</v>
       </c>
@@ -1599,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
         <v>70</v>
       </c>
@@ -1610,7 +1733,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>57</v>
       </c>
@@ -1621,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>71</v>
       </c>
@@ -1632,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>72</v>
       </c>
@@ -1643,7 +1766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>7</v>
       </c>
@@ -1657,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>73</v>
       </c>
@@ -1668,7 +1791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>108</v>
       </c>
@@ -1679,7 +1802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>74</v>
       </c>
@@ -1690,7 +1813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>75</v>
       </c>
@@ -1701,7 +1824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>76</v>
       </c>
@@ -1712,7 +1835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>77</v>
       </c>
@@ -1723,7 +1846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8</v>
       </c>
@@ -1734,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>20</v>
       </c>
@@ -1742,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>21</v>
       </c>
@@ -1750,7 +1873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9</v>
       </c>
@@ -1761,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>103</v>
       </c>
@@ -1769,7 +1892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>104</v>
       </c>
@@ -1777,7 +1900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>105</v>
       </c>
@@ -1785,7 +1908,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>106</v>
       </c>
@@ -1793,7 +1916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>80</v>
       </c>
@@ -1804,7 +1927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>81</v>
       </c>
@@ -1815,7 +1938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
         <v>82</v>
       </c>
@@ -1826,7 +1949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>83</v>
       </c>
@@ -1837,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>84</v>
       </c>
@@ -1846,7 +1969,7 @@
       </c>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>85</v>
       </c>
@@ -1855,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>101</v>
       </c>
@@ -1866,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>86</v>
       </c>
@@ -1877,7 +2000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>87</v>
       </c>
@@ -1888,7 +2011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>88</v>
       </c>
@@ -1899,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>89</v>
       </c>
@@ -1910,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>90</v>
       </c>
@@ -1921,7 +2044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>10</v>
       </c>
@@ -1935,7 +2058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
         <v>81</v>
       </c>
@@ -1944,7 +2067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
         <v>91</v>
       </c>
@@ -1953,7 +2076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
         <v>92</v>
       </c>
@@ -1962,7 +2085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>93</v>
       </c>
@@ -1971,7 +2094,7 @@
       </c>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>94</v>
       </c>
@@ -1980,7 +2103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
         <v>95</v>
       </c>
@@ -1989,7 +2112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="2:4">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
         <v>96</v>
       </c>
@@ -1998,7 +2121,7 @@
       </c>
       <c r="D113" s="3"/>
     </row>
-    <row r="114" spans="2:4">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>97</v>
       </c>
@@ -2007,7 +2130,7 @@
       </c>
       <c r="D114" s="3"/>
     </row>
-    <row r="115" spans="2:4">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>98</v>
       </c>
@@ -2016,7 +2139,7 @@
       </c>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="2:4">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>99</v>
       </c>
@@ -2025,7 +2148,7 @@
       </c>
       <c r="D116" s="3"/>
     </row>
-    <row r="117" spans="2:4">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>100</v>
       </c>
@@ -2046,4 +2169,254 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="9">
+        <v>15000</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="9">
+        <v>20000</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <f>SUM(D18:H18)</f>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>